<commit_message>
Sorted out bug with n splitting in COD code. See very large oscillations at 18.3 kV
</commit_message>
<xml_diff>
--- a/RadialFieldOps_1/RadialFieldScan_1.xlsx
+++ b/RadialFieldOps_1/RadialFieldScan_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/RadialFieldOps_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DDAA187-CC95-B34B-9F23-B12004987713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8639CD02-EED6-EF45-B0F2-C59F85B5DBCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
   </bookViews>
@@ -1175,16 +1175,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1509,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B752E6E-F960-2F47-AC55-2B0104D935A3}">
-  <dimension ref="A2:K14"/>
+  <dimension ref="A2:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1783,6 +1783,98 @@
         <v>2864755.25</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>-0.74199999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="G16">
+        <v>14.8</v>
+      </c>
+      <c r="H16">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E17">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="G17">
+        <v>1.42</v>
+      </c>
+      <c r="H17">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f>ABS(D16-D17)</f>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E18">
+        <f>SQRT(E16^2+E17^2)</f>
+        <v>0.89283873123873836</v>
+      </c>
+      <c r="G18">
+        <f>ABS(G16-G17)</f>
+        <v>13.38</v>
+      </c>
+      <c r="H18">
+        <f>SQRT(H16^2+H17^2)</f>
+        <v>14.235873699917402</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f>D18/E18</f>
+        <v>1.0853023800340675</v>
+      </c>
+      <c r="G19">
+        <f>G18/H18</f>
+        <v>0.93987908870515147</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>0.77299340000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>-0.98535720000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>0.23331389999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>0.37578810000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>-0.7940083</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>1.7285349999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f>STDEV(D29:D34)</f>
+        <v>1.0086629170443522</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>